<commit_message>
create DB and tables
</commit_message>
<xml_diff>
--- a/DB/Data Dictionary_FinalProject.xlsx
+++ b/DB/Data Dictionary_FinalProject.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c02eb9e6f007edb3/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cxxme\source\FinalProject\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC104870999871E65ADE58EA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{07B6BE79-D376-4AE4-A66F-1B21A27480BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4552F3E2-BC72-4817-89CE-BBED7F3656C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Table</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>The time when the game is played</t>
+  </si>
+  <si>
+    <t>PlayTime</t>
   </si>
 </sst>
 </file>
@@ -201,6 +204,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -209,21 +227,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,7 +511,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -520,36 +523,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -571,49 +574,49 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>